<commit_message>
First full test of Landlord(), Renter(), Owner() interactions
</commit_message>
<xml_diff>
--- a/inputs/scenario_test_renters.xlsx
+++ b/inputs/scenario_test_renters.xlsx
@@ -2153,7 +2153,7 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2182,7 +2182,7 @@
         <v>44</v>
       </c>
       <c r="B3">
-        <v>1</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -2198,7 +2198,7 @@
         <v>46</v>
       </c>
       <c r="B5">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Worked on renter eviction & renter home search
</commit_message>
<xml_diff>
--- a/inputs/scenario_test_renters.xlsx
+++ b/inputs/scenario_test_renters.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1040" yWindow="1680" windowWidth="27760" windowHeight="16320" tabRatio="500" activeTab="4"/>
+    <workbookView xWindow="1040" yWindow="1680" windowWidth="27760" windowHeight="16320" tabRatio="500" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="renters" sheetId="5" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="forrent_stock" sheetId="6" r:id="rId4"/>
     <sheet name="human_capital" sheetId="3" r:id="rId5"/>
     <sheet name="financial_capital" sheetId="4" r:id="rId6"/>
+    <sheet name="Sheet1" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="59">
   <si>
     <t>Income</t>
   </si>
@@ -79,9 +80,6 @@
     <t>Mobile Home</t>
   </si>
   <si>
-    <t>None</t>
-  </si>
-  <si>
     <t>Bruce</t>
   </si>
   <si>
@@ -127,42 +125,6 @@
     <t>103 New Ave</t>
   </si>
   <si>
-    <t>104 New Ave</t>
-  </si>
-  <si>
-    <t>105 New Ave</t>
-  </si>
-  <si>
-    <t>106 New Ave</t>
-  </si>
-  <si>
-    <t>107 New Ave</t>
-  </si>
-  <si>
-    <t>108 New Ave</t>
-  </si>
-  <si>
-    <t>109 New Ave</t>
-  </si>
-  <si>
-    <t>110 New Ave</t>
-  </si>
-  <si>
-    <t>111 New Ave</t>
-  </si>
-  <si>
-    <t>112 New Ave</t>
-  </si>
-  <si>
-    <t>113 New Ave</t>
-  </si>
-  <si>
-    <t>114 New Ave</t>
-  </si>
-  <si>
-    <t>115 New Ave</t>
-  </si>
-  <si>
     <t>Contractors</t>
   </si>
   <si>
@@ -248,42 +210,6 @@
   </si>
   <si>
     <t>103 Old Ave</t>
-  </si>
-  <si>
-    <t>104 Old Ave</t>
-  </si>
-  <si>
-    <t>105 Old Ave</t>
-  </si>
-  <si>
-    <t>106 Old Ave</t>
-  </si>
-  <si>
-    <t>107 Old Ave</t>
-  </si>
-  <si>
-    <t>108 Old Ave</t>
-  </si>
-  <si>
-    <t>109 Old Ave</t>
-  </si>
-  <si>
-    <t>110 Old Ave</t>
-  </si>
-  <si>
-    <t>111 Old Ave</t>
-  </si>
-  <si>
-    <t>112 Old Ave</t>
-  </si>
-  <si>
-    <t>113 Old Ave</t>
-  </si>
-  <si>
-    <t>114 Old Ave</t>
-  </si>
-  <si>
-    <t>115 Old Ave</t>
   </si>
 </sst>
 </file>
@@ -601,7 +527,7 @@
   <dimension ref="A1:P5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+      <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -611,7 +537,7 @@
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -650,18 +576,18 @@
         <v>11</v>
       </c>
       <c r="N1" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
       <c r="O1" t="s">
-        <v>57</v>
+        <v>44</v>
       </c>
       <c r="P1" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="B2">
         <v>30000</v>
@@ -673,13 +599,13 @@
         <v>0</v>
       </c>
       <c r="E2" t="s">
-        <v>63</v>
+        <v>50</v>
       </c>
       <c r="F2" t="s">
         <v>14</v>
       </c>
       <c r="G2">
-        <v>100</v>
+        <v>1000</v>
       </c>
       <c r="H2">
         <v>1</v>
@@ -697,21 +623,21 @@
         <v>100000</v>
       </c>
       <c r="M2" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="N2" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="O2" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="P2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="B3">
         <v>100000</v>
@@ -723,13 +649,13 @@
         <v>10000000</v>
       </c>
       <c r="E3" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="F3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G3">
-        <v>100000</v>
+        <v>2500</v>
       </c>
       <c r="H3">
         <v>3</v>
@@ -747,21 +673,21 @@
         <v>10000000</v>
       </c>
       <c r="M3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="N3" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="O3" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="P3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="B4">
         <v>10000</v>
@@ -773,13 +699,13 @@
         <v>0</v>
       </c>
       <c r="E4" t="s">
-        <v>65</v>
+        <v>52</v>
       </c>
       <c r="F4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G4">
-        <v>10</v>
+        <v>750</v>
       </c>
       <c r="H4">
         <v>0</v>
@@ -797,21 +723,21 @@
         <v>10000</v>
       </c>
       <c r="M4" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="N4" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="O4" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="P4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="B5">
         <v>50000</v>
@@ -823,10 +749,10 @@
         <v>550000</v>
       </c>
       <c r="E5" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
       <c r="F5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G5">
         <v>2000</v>
@@ -847,16 +773,16 @@
         <v>800000</v>
       </c>
       <c r="M5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="N5" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="O5" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="P5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -869,7 +795,7 @@
   <dimension ref="A1:P5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -879,7 +805,7 @@
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -918,13 +844,13 @@
         <v>11</v>
       </c>
       <c r="N1" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
       <c r="O1" t="s">
-        <v>57</v>
+        <v>44</v>
       </c>
       <c r="P1" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.2">
@@ -935,7 +861,7 @@
         <v>30000</v>
       </c>
       <c r="C2">
-        <v>10000</v>
+        <v>0</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -947,7 +873,7 @@
         <v>14</v>
       </c>
       <c r="G2">
-        <v>100</v>
+        <v>1500</v>
       </c>
       <c r="H2">
         <v>1</v>
@@ -965,21 +891,21 @@
         <v>100000</v>
       </c>
       <c r="M2" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="N2" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="O2" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="P2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B3">
         <v>100000</v>
@@ -991,13 +917,13 @@
         <v>10000000</v>
       </c>
       <c r="E3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" t="s">
         <v>17</v>
       </c>
-      <c r="F3" t="s">
-        <v>18</v>
-      </c>
       <c r="G3">
-        <v>100000</v>
+        <v>3500</v>
       </c>
       <c r="H3">
         <v>5</v>
@@ -1015,21 +941,21 @@
         <v>10000000</v>
       </c>
       <c r="M3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="N3" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="O3" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="P3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B4">
         <v>10000</v>
@@ -1041,13 +967,13 @@
         <v>0</v>
       </c>
       <c r="E4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G4">
-        <v>10</v>
+        <v>1000</v>
       </c>
       <c r="H4">
         <v>0</v>
@@ -1065,21 +991,21 @@
         <v>10000</v>
       </c>
       <c r="M4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="N4" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="O4" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="P4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B5">
         <v>50000</v>
@@ -1091,13 +1017,13 @@
         <v>550000</v>
       </c>
       <c r="E5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G5">
-        <v>2000</v>
+        <v>3000</v>
       </c>
       <c r="H5">
         <v>4</v>
@@ -1115,16 +1041,16 @@
         <v>800000</v>
       </c>
       <c r="M5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="N5" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="O5" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="P5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -1134,10 +1060,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I17"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1173,7 +1099,7 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B2" t="s">
         <v>14</v>
@@ -1197,15 +1123,15 @@
         <v>99999</v>
       </c>
       <c r="I2" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C3">
         <v>100000</v>
@@ -1226,15 +1152,15 @@
         <v>9999</v>
       </c>
       <c r="I3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C4">
         <v>10</v>
@@ -1255,15 +1181,15 @@
         <v>9999</v>
       </c>
       <c r="I4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C5">
         <v>2000</v>
@@ -1284,355 +1210,7 @@
         <v>800000</v>
       </c>
       <c r="I5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>31</v>
-      </c>
-      <c r="B6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6">
-        <v>100</v>
-      </c>
-      <c r="D6">
-        <v>1</v>
-      </c>
-      <c r="E6">
-        <v>1</v>
-      </c>
-      <c r="F6">
-        <v>700</v>
-      </c>
-      <c r="G6">
-        <v>1920</v>
-      </c>
-      <c r="H6">
-        <v>100000</v>
-      </c>
-      <c r="I6" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>32</v>
-      </c>
-      <c r="B7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7">
-        <v>100000</v>
-      </c>
-      <c r="D7">
-        <v>6</v>
-      </c>
-      <c r="E7">
-        <v>5</v>
-      </c>
-      <c r="F7">
-        <v>5000</v>
-      </c>
-      <c r="G7">
-        <v>1920</v>
-      </c>
-      <c r="H7">
-        <v>10000000</v>
-      </c>
-      <c r="I7" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>33</v>
-      </c>
-      <c r="B8" t="s">
         <v>22</v>
-      </c>
-      <c r="C8">
-        <v>10</v>
-      </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
-      <c r="E8">
-        <v>1</v>
-      </c>
-      <c r="F8">
-        <v>250</v>
-      </c>
-      <c r="G8">
-        <v>1960</v>
-      </c>
-      <c r="H8">
-        <v>9999</v>
-      </c>
-      <c r="I8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>34</v>
-      </c>
-      <c r="B9" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9">
-        <v>2000</v>
-      </c>
-      <c r="D9">
-        <v>4</v>
-      </c>
-      <c r="E9">
-        <v>2</v>
-      </c>
-      <c r="F9">
-        <v>2000</v>
-      </c>
-      <c r="G9">
-        <v>2010</v>
-      </c>
-      <c r="H9">
-        <v>800000</v>
-      </c>
-      <c r="I9" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>35</v>
-      </c>
-      <c r="B10" t="s">
-        <v>14</v>
-      </c>
-      <c r="C10">
-        <v>100</v>
-      </c>
-      <c r="D10">
-        <v>1</v>
-      </c>
-      <c r="E10">
-        <v>1</v>
-      </c>
-      <c r="F10">
-        <v>700</v>
-      </c>
-      <c r="G10">
-        <v>1920</v>
-      </c>
-      <c r="H10">
-        <v>100000</v>
-      </c>
-      <c r="I10" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>36</v>
-      </c>
-      <c r="B11" t="s">
-        <v>18</v>
-      </c>
-      <c r="C11">
-        <v>100000</v>
-      </c>
-      <c r="D11">
-        <v>6</v>
-      </c>
-      <c r="E11">
-        <v>5</v>
-      </c>
-      <c r="F11">
-        <v>5000</v>
-      </c>
-      <c r="G11">
-        <v>1920</v>
-      </c>
-      <c r="H11">
-        <v>10000000</v>
-      </c>
-      <c r="I11" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>37</v>
-      </c>
-      <c r="B12" t="s">
-        <v>22</v>
-      </c>
-      <c r="C12">
-        <v>10</v>
-      </c>
-      <c r="D12">
-        <v>0</v>
-      </c>
-      <c r="E12">
-        <v>1</v>
-      </c>
-      <c r="F12">
-        <v>250</v>
-      </c>
-      <c r="G12">
-        <v>1960</v>
-      </c>
-      <c r="H12">
-        <v>10000</v>
-      </c>
-      <c r="I12" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>38</v>
-      </c>
-      <c r="B13" t="s">
-        <v>18</v>
-      </c>
-      <c r="C13">
-        <v>2000</v>
-      </c>
-      <c r="D13">
-        <v>4</v>
-      </c>
-      <c r="E13">
-        <v>2</v>
-      </c>
-      <c r="F13">
-        <v>2000</v>
-      </c>
-      <c r="G13">
-        <v>2010</v>
-      </c>
-      <c r="H13">
-        <v>800000</v>
-      </c>
-      <c r="I13" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>39</v>
-      </c>
-      <c r="B14" t="s">
-        <v>14</v>
-      </c>
-      <c r="C14">
-        <v>100</v>
-      </c>
-      <c r="D14">
-        <v>1</v>
-      </c>
-      <c r="E14">
-        <v>1</v>
-      </c>
-      <c r="F14">
-        <v>700</v>
-      </c>
-      <c r="G14">
-        <v>1920</v>
-      </c>
-      <c r="H14">
-        <v>100000</v>
-      </c>
-      <c r="I14" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>40</v>
-      </c>
-      <c r="B15" t="s">
-        <v>18</v>
-      </c>
-      <c r="C15">
-        <v>100000</v>
-      </c>
-      <c r="D15">
-        <v>6</v>
-      </c>
-      <c r="E15">
-        <v>5</v>
-      </c>
-      <c r="F15">
-        <v>5000</v>
-      </c>
-      <c r="G15">
-        <v>1920</v>
-      </c>
-      <c r="H15">
-        <v>10000000</v>
-      </c>
-      <c r="I15" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>41</v>
-      </c>
-      <c r="B16" t="s">
-        <v>22</v>
-      </c>
-      <c r="C16">
-        <v>10</v>
-      </c>
-      <c r="D16">
-        <v>0</v>
-      </c>
-      <c r="E16">
-        <v>1</v>
-      </c>
-      <c r="F16">
-        <v>250</v>
-      </c>
-      <c r="G16">
-        <v>1960</v>
-      </c>
-      <c r="H16">
-        <v>10000</v>
-      </c>
-      <c r="I16" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>42</v>
-      </c>
-      <c r="B17" t="s">
-        <v>18</v>
-      </c>
-      <c r="C17">
-        <v>2000</v>
-      </c>
-      <c r="D17">
-        <v>4</v>
-      </c>
-      <c r="E17">
-        <v>2</v>
-      </c>
-      <c r="F17">
-        <v>2000</v>
-      </c>
-      <c r="G17">
-        <v>2010</v>
-      </c>
-      <c r="H17">
-        <v>800000</v>
-      </c>
-      <c r="I17" t="s">
-        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -1642,10 +1220,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I17"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1681,10 +1259,10 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
       <c r="B2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C2">
         <v>100</v>
@@ -1705,15 +1283,15 @@
         <v>99999</v>
       </c>
       <c r="I2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>69</v>
+        <v>56</v>
       </c>
       <c r="B3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C3">
         <v>100000</v>
@@ -1734,15 +1312,15 @@
         <v>9999</v>
       </c>
       <c r="I3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="B4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C4">
         <v>10</v>
@@ -1763,15 +1341,15 @@
         <v>9999</v>
       </c>
       <c r="I4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C5">
         <v>2000</v>
@@ -1792,355 +1370,7 @@
         <v>800000</v>
       </c>
       <c r="I5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>72</v>
-      </c>
-      <c r="B6" t="s">
-        <v>22</v>
-      </c>
-      <c r="C6">
-        <v>100</v>
-      </c>
-      <c r="D6">
-        <v>1</v>
-      </c>
-      <c r="E6">
-        <v>1</v>
-      </c>
-      <c r="F6">
-        <v>700</v>
-      </c>
-      <c r="G6">
-        <v>1920</v>
-      </c>
-      <c r="H6">
-        <v>100000</v>
-      </c>
-      <c r="I6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>73</v>
-      </c>
-      <c r="B7" t="s">
         <v>18</v>
-      </c>
-      <c r="C7">
-        <v>100000</v>
-      </c>
-      <c r="D7">
-        <v>2</v>
-      </c>
-      <c r="E7">
-        <v>2</v>
-      </c>
-      <c r="F7">
-        <v>5000</v>
-      </c>
-      <c r="G7">
-        <v>1920</v>
-      </c>
-      <c r="H7">
-        <v>10000000</v>
-      </c>
-      <c r="I7" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>74</v>
-      </c>
-      <c r="B8" t="s">
-        <v>22</v>
-      </c>
-      <c r="C8">
-        <v>10</v>
-      </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
-      <c r="E8">
-        <v>1</v>
-      </c>
-      <c r="F8">
-        <v>250</v>
-      </c>
-      <c r="G8">
-        <v>1960</v>
-      </c>
-      <c r="H8">
-        <v>9999</v>
-      </c>
-      <c r="I8" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>75</v>
-      </c>
-      <c r="B9" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9">
-        <v>2000</v>
-      </c>
-      <c r="D9">
-        <v>3</v>
-      </c>
-      <c r="E9">
-        <v>2</v>
-      </c>
-      <c r="F9">
-        <v>2000</v>
-      </c>
-      <c r="G9">
-        <v>2010</v>
-      </c>
-      <c r="H9">
-        <v>800000</v>
-      </c>
-      <c r="I9" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>76</v>
-      </c>
-      <c r="B10" t="s">
-        <v>22</v>
-      </c>
-      <c r="C10">
-        <v>100</v>
-      </c>
-      <c r="D10">
-        <v>1</v>
-      </c>
-      <c r="E10">
-        <v>1</v>
-      </c>
-      <c r="F10">
-        <v>700</v>
-      </c>
-      <c r="G10">
-        <v>1920</v>
-      </c>
-      <c r="H10">
-        <v>100000</v>
-      </c>
-      <c r="I10" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>77</v>
-      </c>
-      <c r="B11" t="s">
-        <v>18</v>
-      </c>
-      <c r="C11">
-        <v>100000</v>
-      </c>
-      <c r="D11">
-        <v>3</v>
-      </c>
-      <c r="E11">
-        <v>3</v>
-      </c>
-      <c r="F11">
-        <v>5000</v>
-      </c>
-      <c r="G11">
-        <v>1920</v>
-      </c>
-      <c r="H11">
-        <v>10000000</v>
-      </c>
-      <c r="I11" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>78</v>
-      </c>
-      <c r="B12" t="s">
-        <v>22</v>
-      </c>
-      <c r="C12">
-        <v>10</v>
-      </c>
-      <c r="D12">
-        <v>0</v>
-      </c>
-      <c r="E12">
-        <v>1</v>
-      </c>
-      <c r="F12">
-        <v>250</v>
-      </c>
-      <c r="G12">
-        <v>1960</v>
-      </c>
-      <c r="H12">
-        <v>10000</v>
-      </c>
-      <c r="I12" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>79</v>
-      </c>
-      <c r="B13" t="s">
-        <v>18</v>
-      </c>
-      <c r="C13">
-        <v>2000</v>
-      </c>
-      <c r="D13">
-        <v>2</v>
-      </c>
-      <c r="E13">
-        <v>2</v>
-      </c>
-      <c r="F13">
-        <v>2000</v>
-      </c>
-      <c r="G13">
-        <v>2010</v>
-      </c>
-      <c r="H13">
-        <v>800000</v>
-      </c>
-      <c r="I13" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>80</v>
-      </c>
-      <c r="B14" t="s">
-        <v>22</v>
-      </c>
-      <c r="C14">
-        <v>100</v>
-      </c>
-      <c r="D14">
-        <v>1</v>
-      </c>
-      <c r="E14">
-        <v>1</v>
-      </c>
-      <c r="F14">
-        <v>700</v>
-      </c>
-      <c r="G14">
-        <v>1920</v>
-      </c>
-      <c r="H14">
-        <v>100000</v>
-      </c>
-      <c r="I14" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>81</v>
-      </c>
-      <c r="B15" t="s">
-        <v>18</v>
-      </c>
-      <c r="C15">
-        <v>100000</v>
-      </c>
-      <c r="D15">
-        <v>2</v>
-      </c>
-      <c r="E15">
-        <v>2</v>
-      </c>
-      <c r="F15">
-        <v>5000</v>
-      </c>
-      <c r="G15">
-        <v>1920</v>
-      </c>
-      <c r="H15">
-        <v>10000000</v>
-      </c>
-      <c r="I15" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>82</v>
-      </c>
-      <c r="B16" t="s">
-        <v>22</v>
-      </c>
-      <c r="C16">
-        <v>10</v>
-      </c>
-      <c r="D16">
-        <v>0</v>
-      </c>
-      <c r="E16">
-        <v>1</v>
-      </c>
-      <c r="F16">
-        <v>250</v>
-      </c>
-      <c r="G16">
-        <v>1960</v>
-      </c>
-      <c r="H16">
-        <v>10000</v>
-      </c>
-      <c r="I16" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>83</v>
-      </c>
-      <c r="B17" t="s">
-        <v>22</v>
-      </c>
-      <c r="C17">
-        <v>2000</v>
-      </c>
-      <c r="D17">
-        <v>2</v>
-      </c>
-      <c r="E17">
-        <v>2</v>
-      </c>
-      <c r="F17">
-        <v>2000</v>
-      </c>
-      <c r="G17">
-        <v>2010</v>
-      </c>
-      <c r="H17">
-        <v>800000</v>
-      </c>
-      <c r="I17" t="s">
-        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -2152,8 +1382,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2163,15 +1393,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="B1" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="B2">
         <v>40</v>
@@ -2179,7 +1409,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="B3">
         <v>20</v>
@@ -2187,7 +1417,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="B4">
         <v>40</v>
@@ -2195,7 +1425,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="B5">
         <v>4</v>
@@ -2203,7 +1433,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="B6">
         <v>40</v>
@@ -2211,7 +1441,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="B7">
         <v>40</v>
@@ -2219,7 +1449,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="B8">
         <v>100</v>
@@ -2245,15 +1475,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="B1" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>50</v>
+        <v>37</v>
       </c>
       <c r="B2">
         <v>2000000</v>
@@ -2261,7 +1491,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="B3">
         <v>35000000</v>
@@ -2270,4 +1500,18 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J27" sqref="J27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Feature improvements for renters() class
</commit_message>
<xml_diff>
--- a/inputs/scenario_test_renters.xlsx
+++ b/inputs/scenario_test_renters.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27715"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27815"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1040" yWindow="1680" windowWidth="27760" windowHeight="16320" tabRatio="500" activeTab="6"/>
+    <workbookView xWindow="1040" yWindow="1680" windowWidth="27760" windowHeight="16320" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="renters" sheetId="5" r:id="rId1"/>
@@ -89,9 +89,6 @@
     <t>Single Family Dwelling</t>
   </si>
   <si>
-    <t>Slight</t>
-  </si>
-  <si>
     <t>Selena</t>
   </si>
   <si>
@@ -110,9 +107,6 @@
     <t>26000 Out There Lane</t>
   </si>
   <si>
-    <t>Moderate</t>
-  </si>
-  <si>
     <t>100 New Ave</t>
   </si>
   <si>
@@ -210,6 +204,12 @@
   </si>
   <si>
     <t>103 Old Ave</t>
+  </si>
+  <si>
+    <t>Extensive</t>
+  </si>
+  <si>
+    <t>None</t>
   </si>
 </sst>
 </file>
@@ -526,8 +526,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -537,7 +537,7 @@
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -576,18 +576,18 @@
         <v>11</v>
       </c>
       <c r="N1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="O1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="P1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B2">
         <v>30000</v>
@@ -599,7 +599,7 @@
         <v>0</v>
       </c>
       <c r="E2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F2" t="s">
         <v>14</v>
@@ -623,13 +623,13 @@
         <v>100000</v>
       </c>
       <c r="M2" t="s">
-        <v>22</v>
+        <v>57</v>
       </c>
       <c r="N2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="O2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="P2" t="s">
         <v>17</v>
@@ -637,7 +637,7 @@
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B3">
         <v>100000</v>
@@ -649,7 +649,7 @@
         <v>10000000</v>
       </c>
       <c r="E3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F3" t="s">
         <v>17</v>
@@ -673,13 +673,13 @@
         <v>10000000</v>
       </c>
       <c r="M3" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="N3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="O3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="P3" t="s">
         <v>17</v>
@@ -687,7 +687,7 @@
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B4">
         <v>10000</v>
@@ -699,10 +699,10 @@
         <v>0</v>
       </c>
       <c r="E4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G4">
         <v>750</v>
@@ -723,21 +723,21 @@
         <v>10000</v>
       </c>
       <c r="M4" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="N4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="O4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="P4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B5">
         <v>50000</v>
@@ -749,7 +749,7 @@
         <v>550000</v>
       </c>
       <c r="E5" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F5" t="s">
         <v>17</v>
@@ -773,13 +773,13 @@
         <v>800000</v>
       </c>
       <c r="M5" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="N5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="O5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="P5" t="s">
         <v>17</v>
@@ -795,7 +795,7 @@
   <dimension ref="A1:P5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -805,7 +805,7 @@
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -844,13 +844,13 @@
         <v>11</v>
       </c>
       <c r="N1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="O1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="P1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.2">
@@ -891,13 +891,13 @@
         <v>100000</v>
       </c>
       <c r="M2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="N2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="O2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="P2" t="s">
         <v>17</v>
@@ -914,7 +914,7 @@
         <v>1000000</v>
       </c>
       <c r="D3">
-        <v>10000000</v>
+        <v>0.85</v>
       </c>
       <c r="E3" t="s">
         <v>16</v>
@@ -941,13 +941,13 @@
         <v>10000000</v>
       </c>
       <c r="M3" t="s">
-        <v>18</v>
+        <v>58</v>
       </c>
       <c r="N3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="O3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="P3" t="s">
         <v>17</v>
@@ -955,7 +955,7 @@
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B4">
         <v>10000</v>
@@ -967,7 +967,7 @@
         <v>0</v>
       </c>
       <c r="E4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F4" t="s">
         <v>17</v>
@@ -991,13 +991,13 @@
         <v>10000</v>
       </c>
       <c r="M4" t="s">
-        <v>22</v>
+        <v>58</v>
       </c>
       <c r="N4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="O4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="P4" t="s">
         <v>17</v>
@@ -1005,7 +1005,7 @@
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B5">
         <v>50000</v>
@@ -1014,10 +1014,10 @@
         <v>1000</v>
       </c>
       <c r="D5">
-        <v>550000</v>
+        <v>0.85</v>
       </c>
       <c r="E5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F5" t="s">
         <v>17</v>
@@ -1041,13 +1041,13 @@
         <v>800000</v>
       </c>
       <c r="M5" t="s">
-        <v>25</v>
+        <v>58</v>
       </c>
       <c r="N5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="O5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="P5" t="s">
         <v>17</v>
@@ -1063,7 +1063,7 @@
   <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1099,7 +1099,7 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B2" t="s">
         <v>14</v>
@@ -1123,12 +1123,12 @@
         <v>99999</v>
       </c>
       <c r="I2" t="s">
-        <v>18</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B3" t="s">
         <v>17</v>
@@ -1152,15 +1152,15 @@
         <v>9999</v>
       </c>
       <c r="I3" t="s">
-        <v>22</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C4">
         <v>10</v>
@@ -1181,12 +1181,12 @@
         <v>9999</v>
       </c>
       <c r="I4" t="s">
-        <v>22</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B5" t="s">
         <v>17</v>
@@ -1210,7 +1210,7 @@
         <v>800000</v>
       </c>
       <c r="I5" t="s">
-        <v>22</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -1223,7 +1223,7 @@
   <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="I2" sqref="I2:I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1259,10 +1259,10 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B2" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="C2">
         <v>100</v>
@@ -1283,12 +1283,12 @@
         <v>99999</v>
       </c>
       <c r="I2" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B3" t="s">
         <v>17</v>
@@ -1312,15 +1312,15 @@
         <v>9999</v>
       </c>
       <c r="I3" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C4">
         <v>10</v>
@@ -1341,12 +1341,12 @@
         <v>9999</v>
       </c>
       <c r="I4" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B5" t="s">
         <v>17</v>
@@ -1370,7 +1370,7 @@
         <v>800000</v>
       </c>
       <c r="I5" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -1393,15 +1393,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B2">
         <v>40</v>
@@ -1409,7 +1409,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B3">
         <v>20</v>
@@ -1417,7 +1417,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B4">
         <v>40</v>
@@ -1425,7 +1425,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B5">
         <v>4</v>
@@ -1433,7 +1433,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B6">
         <v>40</v>
@@ -1441,7 +1441,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B7">
         <v>40</v>
@@ -1449,7 +1449,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B8">
         <v>100</v>
@@ -1475,15 +1475,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B2">
         <v>2000000</v>
@@ -1491,7 +1491,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B3">
         <v>35000000</v>
@@ -1506,7 +1506,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J27" sqref="J27"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Integrating Derek's viz notebooks into my branch
</commit_message>
<xml_diff>
--- a/inputs/scenario_test_renters.xlsx
+++ b/inputs/scenario_test_renters.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27815"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28016"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1040" yWindow="1680" windowWidth="27760" windowHeight="16320" tabRatio="500"/>
+    <workbookView xWindow="1040" yWindow="1680" windowWidth="27760" windowHeight="16320" tabRatio="500" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="renters" sheetId="5" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="60">
   <si>
     <t>Income</t>
   </si>
@@ -210,6 +210,9 @@
   </si>
   <si>
     <t>None</t>
+  </si>
+  <si>
+    <t>Moderate</t>
   </si>
 </sst>
 </file>
@@ -526,7 +529,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
@@ -795,7 +798,7 @@
   <dimension ref="A1:P5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -861,7 +864,7 @@
         <v>30000</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>5000</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -882,7 +885,7 @@
         <v>1</v>
       </c>
       <c r="J2">
-        <v>700</v>
+        <v>1100</v>
       </c>
       <c r="K2">
         <v>1920</v>
@@ -926,7 +929,7 @@
         <v>3500</v>
       </c>
       <c r="H3">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I3">
         <v>5</v>
@@ -941,7 +944,7 @@
         <v>10000000</v>
       </c>
       <c r="M3" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="N3" t="s">
         <v>41</v>
@@ -961,7 +964,7 @@
         <v>10000</v>
       </c>
       <c r="C4">
-        <v>100</v>
+        <v>2500</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -976,13 +979,13 @@
         <v>1000</v>
       </c>
       <c r="H4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I4">
         <v>1</v>
       </c>
       <c r="J4">
-        <v>250</v>
+        <v>1200</v>
       </c>
       <c r="K4">
         <v>1960</v>
@@ -991,7 +994,7 @@
         <v>10000</v>
       </c>
       <c r="M4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="N4" t="s">
         <v>41</v>
@@ -1026,7 +1029,7 @@
         <v>3000</v>
       </c>
       <c r="H5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I5">
         <v>2</v>
@@ -1041,7 +1044,7 @@
         <v>800000</v>
       </c>
       <c r="M5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="N5" t="s">
         <v>41</v>
@@ -1382,8 +1385,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1404,7 +1407,7 @@
         <v>28</v>
       </c>
       <c r="B2">
-        <v>40</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -1412,7 +1415,7 @@
         <v>29</v>
       </c>
       <c r="B3">
-        <v>20</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -1420,7 +1423,7 @@
         <v>30</v>
       </c>
       <c r="B4">
-        <v>40</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -1452,7 +1455,7 @@
         <v>34</v>
       </c>
       <c r="B8">
-        <v>100</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Refactored to fully implement RecoveryProgram() class structure, including RecoveryProgram.process()
programs.py, technical.py, funding.py
</commit_message>
<xml_diff>
--- a/inputs/scenario_test_renters.xlsx
+++ b/inputs/scenario_test_renters.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28016"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28109"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1040" yWindow="1680" windowWidth="27760" windowHeight="16320" tabRatio="500" activeTab="4"/>
+    <workbookView xWindow="1040" yWindow="1680" windowWidth="27760" windowHeight="16320" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="renters" sheetId="5" r:id="rId1"/>
@@ -797,8 +797,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M5" sqref="M5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -914,7 +914,7 @@
         <v>100000</v>
       </c>
       <c r="C3">
-        <v>1000000</v>
+        <v>250000</v>
       </c>
       <c r="D3">
         <v>0.85</v>
@@ -1385,8 +1385,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>